<commit_message>
#3 resolve and 1.1.1 release
</commit_message>
<xml_diff>
--- a/bin/Debug/Interior_editor.xlsx
+++ b/bin/Debug/Interior_editor.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Car Editor\Car Editor\Car Editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33DE8763-B33C-4EB5-960D-386DCD7E060E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B4DA7E-BDD9-435F-B598-8019137E16C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9AE4505A-1977-4BEB-926A-0F65BFBC3A67}"/>
   </bookViews>
@@ -33,6 +33,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,62 +421,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B602692-4F60-4A9D-B138-F26F361DF22F}">
-  <dimension ref="G2:I8"/>
+  <dimension ref="G2:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
     <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="7:9" ht="60">
+    <row r="2" spans="7:10" ht="60">
       <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H2" t="str">
-        <f>RIGHT(G2,LEN(G2)-SEARCH(",",G2,1))</f>
-        <v xml:space="preserve"> -47.3793, -54.6411, 221.6433</v>
-      </c>
       <c r="I2" t="str">
         <f>RIGHT(H2,18)</f>
-        <v>-54.6411, 221.6433</v>
+        <v/>
       </c>
     </row>
-    <row r="3" spans="7:9">
-      <c r="G3" t="str">
-        <f>LEFT(G2,10)</f>
+    <row r="3" spans="7:10">
+      <c r="G3" t="str" cm="1">
+        <f t="array" ref="G3:J3">_xlfn.TEXTSPLIT(G2,",",",",1)</f>
         <v>-1466.0389</v>
       </c>
       <c r="H3" t="str">
-        <f>LEFT(H2,9)</f>
         <v xml:space="preserve"> -47.3793</v>
       </c>
       <c r="I3" t="str">
-        <f>LEFT(I2,8)</f>
-        <v>-54.6411</v>
+        <v xml:space="preserve"> -54.6411</v>
+      </c>
+      <c r="J3" t="str">
+        <v xml:space="preserve"> 221.6433</v>
       </c>
     </row>
-    <row r="6" spans="7:9">
+    <row r="6" spans="7:10">
       <c r="G6" t="str">
         <f>_xlfn.CONCAT("       x = ",G3,",")</f>
         <v xml:space="preserve">       x = -1466.0389,</v>
       </c>
     </row>
-    <row r="7" spans="7:9">
+    <row r="7" spans="7:10">
       <c r="G7" t="str">
         <f>_xlfn.CONCAT("       y = ",H3,",")</f>
         <v xml:space="preserve">       y =  -47.3793,</v>
       </c>
     </row>
-    <row r="8" spans="7:9">
+    <row r="8" spans="7:10">
       <c r="G8" t="str">
         <f>_xlfn.CONCAT("       z = ",I3,)</f>
-        <v xml:space="preserve">       z = -54.6411</v>
+        <v xml:space="preserve">       z =  -54.6411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>